<commit_message>
feat: make weak depend on spring
</commit_message>
<xml_diff>
--- a/shared/excel/tmp/kycTask.xlsx
+++ b/shared/excel/tmp/kycTask.xlsx
@@ -349,7 +349,7 @@
         <v>36161.0</v>
       </c>
       <c r="Y2" t="n" s="7">
-        <v>45598.56322496528</v>
+        <v>45601.90549978009</v>
       </c>
     </row>
     <row r="3">
@@ -404,7 +404,7 @@
         <v>401404.0</v>
       </c>
       <c r="Y4" t="n" s="7">
-        <v>45598.56322496528</v>
+        <v>45601.90549978009</v>
       </c>
     </row>
   </sheetData>

</xml_diff>